<commit_message>
bump: updating KICS KPI Statistics of new release
</commit_message>
<xml_diff>
--- a/KICS-KPIs-over-time.xlsx
+++ b/KICS-KPIs-over-time.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC103"/>
+  <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7680,6 +7680,131 @@
         <v>64</v>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2023/07/17</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>v1.7.3</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>2492</v>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>43812</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>2063442</v>
+      </c>
+      <c r="H104" t="n">
+        <v>1639</v>
+      </c>
+      <c r="I104" t="n">
+        <v>252</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K104" t="n">
+        <v>2133</v>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="N104" t="n">
+        <v>42</v>
+      </c>
+      <c r="O104" t="n">
+        <v>315</v>
+      </c>
+      <c r="P104" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q104" t="n">
+        <v>73</v>
+      </c>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="T104" t="inlineStr">
+        <is>
+          <t>1084</t>
+        </is>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="V104" t="n">
+        <v>7166</v>
+      </c>
+      <c r="W104" t="n">
+        <v>64</v>
+      </c>
+      <c r="X104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Y104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Z104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AA104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AB104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AC104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>